<commit_message>
Added STD, Update SPPP, and Progress Report
</commit_message>
<xml_diff>
--- a/Doc/iteration1/CS673_ProgressReport_team2.xlsx
+++ b/Doc/iteration1/CS673_ProgressReport_team2.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="127">
   <si>
     <t xml:space="preserve">This report has 1 group iteration progress summary sheet to be filled at the end of each iteration by the team leader, 
 1 project ontribution sheet to be filled by everyone at the end of the semester, and 1 weekly report sheet per student. </t>
@@ -312,6 +312,21 @@
     <t>5 - caught up</t>
   </si>
   <si>
+    <t>5/24 - 05/31</t>
+  </si>
+  <si>
+    <t>0 - did more research about the different testing frameworks and which one would be best with our current stack, learned React components unit testing
+4 - Set up Jest testing framework for front-end + back-end</t>
+  </si>
+  <si>
+    <t>Did STD
+Updated SPPP</t>
+  </si>
+  <si>
+    <t>Write tests
+Setup Continuous Testing</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -395,7 +410,10 @@
 Studied distributed system concepts and design patterns and analyze our application for design patterns</t>
   </si>
   <si>
-    <t>--</t>
+    <t xml:space="preserve">5 All team members were not familiar with each others work and stack so we spent some time syncing on these items5 </t>
+  </si>
+  <si>
+    <t>5 - Adjusted scheduled and meeting plans accordingly to allow for extra time</t>
   </si>
   <si>
     <t xml:space="preserve">2 - Add polishing touches and CSS to frontend and focus on backend optimization
@@ -508,9 +526,6 @@
 </t>
   </si>
   <si>
-    <t>5/24 - 05/31</t>
-  </si>
-  <si>
     <t>0 - read styled-components documentation, study MVC architecture, study sequence diagrams
 1 - Update requirements in SPP: add color system, followup alert and customizable configurations. Rewrite Usability
 2 - degin UI mockups and write SDD UI design section 
@@ -610,14 +625,16 @@
 7-demo for the iteration1 project</t>
   </si>
   <si>
-    <t>1. SDD: class digram part and UI design</t>
+    <t>1. SDD: class digram part and UI design
+2. demo video</t>
   </si>
   <si>
     <t>1.did not manage my time well because this week is the first week of my summer intern 
 2.did not communcate with teammember well on backend parts</t>
   </si>
   <si>
-    <t>arrange my time well and communate with team member more</t>
+    <t>1.arrange my time well and communate with team member more
+2. Weekly meeting will be in the early week day.</t>
   </si>
   <si>
     <t xml:space="preserve">-Work on backend
@@ -8359,11 +8376,11 @@
         <v>52</v>
       </c>
       <c r="C4" s="19">
-        <f t="shared" ref="C4:C5" si="1">D4+E4</f>
+        <f t="shared" ref="C4:C6" si="1">D4+E4</f>
         <v>10</v>
       </c>
       <c r="D4" s="19">
-        <f t="shared" ref="D4:D5" si="2">sum(G4:N4)</f>
+        <f t="shared" ref="D4:D6" si="2">sum(G4:N4)</f>
         <v>6</v>
       </c>
       <c r="E4" s="22">
@@ -8456,19 +8473,49 @@
       <c r="T5" s="6"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="A6" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="23">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D6" s="23">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E6" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="L6" s="7"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="S6" s="7">
+        <v>20.0</v>
+      </c>
       <c r="T6" s="6"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -12740,7 +12787,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -12836,7 +12883,7 @@
         <v>4.0</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G4" s="22">
         <v>5.0</v>
@@ -12853,16 +12900,16 @@
       </c>
       <c r="N4" s="19"/>
       <c r="O4" s="22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="P4" s="22" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="22" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="R4" s="22" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="S4" s="22">
         <v>10.0</v>
@@ -12887,7 +12934,7 @@
         <v>24.0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G5" s="7">
         <v>5.0</v>
@@ -12914,16 +12961,16 @@
         <v>0.0</v>
       </c>
       <c r="O5" s="22" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="S5" s="7">
         <v>12.0</v>
@@ -12935,7 +12982,7 @@
         <v>3.0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C6" s="8">
         <v>12.0</v>
@@ -12948,7 +12995,7 @@
         <v>24.0</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G6" s="7">
         <v>6.0</v>
@@ -12975,16 +13022,16 @@
         <v>0.0</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="S6" s="7">
         <v>8.0</v>
@@ -17263,7 +17310,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -17367,7 +17414,7 @@
         <v>4.0</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G4" s="22">
         <v>1.0</v>
@@ -17388,14 +17435,14 @@
         <v>0.5</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="P4" s="22">
         <v>1.0</v>
       </c>
       <c r="Q4" s="19"/>
       <c r="R4" s="22" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="S4" s="22">
         <v>8.0</v>
@@ -22143,7 +22190,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -22247,7 +22294,7 @@
         <v>4.0</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="G4" s="22">
         <v>5.0</v>
@@ -22266,16 +22313,16 @@
         <v>0.5</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="P4" s="22" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="Q4" s="22" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="R4" s="22" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="S4" s="22">
         <v>10.0</v>
@@ -22293,7 +22340,7 @@
         <v>2.0</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C5" s="23">
         <f t="shared" si="1"/>
@@ -22307,7 +22354,7 @@
         <v>2.0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G5" s="7">
         <v>3.0</v>
@@ -22326,16 +22373,16 @@
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="7" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="S5" s="7">
         <v>12.0</v>
@@ -22349,7 +22396,7 @@
         <v>3.0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="C6" s="23">
         <f t="shared" si="1"/>
@@ -22363,7 +22410,7 @@
         <v>2.5</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G6" s="7">
         <v>3.0</v>
@@ -22386,16 +22433,16 @@
         <v>0.5</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="S6" s="7">
         <v>15.0</v>
@@ -27103,7 +27150,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -27207,7 +27254,7 @@
         <v>4.0</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G4" s="22">
         <v>2.0</v>
@@ -27224,16 +27271,16 @@
       </c>
       <c r="N4" s="19"/>
       <c r="O4" s="22" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="P4" s="22" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="Q4" s="22" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="R4" s="22" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="S4" s="22">
         <v>15.0</v>
@@ -27251,7 +27298,7 @@
         <v>2.0</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C5" s="19">
         <f t="shared" si="1"/>
@@ -27265,7 +27312,7 @@
         <v>2.0</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="G5" s="22">
         <v>2.0</v>
@@ -27287,13 +27334,13 @@
       <c r="N5" s="19"/>
       <c r="O5" s="22"/>
       <c r="P5" s="22" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="Q5" s="22" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="R5" s="22" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="S5" s="22">
         <v>20.0</v>
@@ -27307,21 +27354,21 @@
         <v>3.0</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C6" s="19">
         <f t="shared" si="1"/>
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="D6" s="19">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="E6" s="22">
         <v>2.5</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G6" s="22">
         <v>3.0</v>
@@ -27338,18 +27385,20 @@
       <c r="M6" s="22">
         <v>0.5</v>
       </c>
-      <c r="N6" s="19"/>
+      <c r="N6" s="22">
+        <v>0.5</v>
+      </c>
       <c r="O6" s="22" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="Q6" s="22" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="R6" s="22" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="S6" s="22">
         <v>15.0</v>

</xml_diff>